<commit_message>
changed email address in test data file
</commit_message>
<xml_diff>
--- a/Data Files/TestData.xlsx
+++ b/Data Files/TestData.xlsx
@@ -81,7 +81,7 @@
     <t>User Sign Up Successful</t>
   </si>
   <si>
-    <t>test8@gmail.com</t>
+    <t>test9@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -412,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>